<commit_message>
【 Project - Basic calculator 】 Document update, naming revise and remove unecessary code
</commit_message>
<xml_diff>
--- a/Project - Basic_calculator/Basic calculator.xlsx
+++ b/Project - Basic_calculator/Basic calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\intelFPGA_lite\18.1\Digital-Clock\Project - Basic_calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576FD536-6EA5-4024-8C28-1368BB56DE46}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D355CA5D-CB6A-47E5-B95C-838947723A1D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{E96232D1-EBEC-446B-8C68-089EF9F142DF}"/>
   </bookViews>
@@ -521,88 +521,6 @@
             <a:rPr lang="en-MY" sz="1100" baseline="0"/>
             <a:t>one</a:t>
           </a:r>
-          <a:endParaRPr lang="en-MY" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>93196</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>97919</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>150469</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>157451</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Speech Bubble: Rectangle 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F52702B4-E9F2-4E64-86B1-4A870186932B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7424162" y="3336419"/>
-          <a:ext cx="1890014" cy="1012032"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 79888"/>
-            <a:gd name="adj2" fmla="val 275735"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-MY" sz="1100"/>
-            <a:t>equal</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-MY" sz="1100"/>
-            <a:t>during this slide switch was on,</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-MY" sz="1100" baseline="0"/>
-            <a:t> press the button 1 will generate result</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-MY" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
           <a:endParaRPr lang="en-MY" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -1207,6 +1125,224 @@
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-MY" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>137948</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>59121</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>164224</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADE27B1A-FE45-426C-8852-CFC7C5A592F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9544707" y="6424448"/>
+          <a:ext cx="899948" cy="216776"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF00FF"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-MY" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>605576</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>45368</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>51934</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>104900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Speech Bubble: Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F52702B4-E9F2-4E64-86B1-4A870186932B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5492886" y="2521868"/>
+          <a:ext cx="1890014" cy="1012032"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 182419"/>
+            <a:gd name="adj2" fmla="val 368554"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-MY" sz="1100"/>
+            <a:t>equal</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-MY" sz="1100"/>
+            <a:t>during this slide switch was on,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-MY" sz="1100" baseline="0"/>
+            <a:t> press the button 1 will generate result</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-MY" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-MY" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>14451</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1312</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>68029</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>60844</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Speech Bubble: Rectangle 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE8344AF-0FB4-488F-B0DF-1B7F1E8107C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12843641" y="4954312"/>
+          <a:ext cx="1886319" cy="1012032"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -176442"/>
+            <a:gd name="adj2" fmla="val 103443"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-MY" sz="1100"/>
+            <a:t>State indicator</a:t>
+          </a:r>
+        </a:p>
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr lang="en-MY" sz="1100"/>
@@ -8641,8 +8777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33404A68-2D35-4971-8A15-DB25450B44DE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="V48" sqref="V48"/>
+    <sheetView tabSelected="1" topLeftCell="F19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="V35" sqref="V35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>